<commit_message>
wip, fix ranks and scores
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/Score-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/Score-A4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/owlcms4/owlcms/src/main/resources/templates/competitionResults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4C2A0-898C-5442-985A-A04F6F5B36DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5501B7BC-01B5-4F93-9A13-521C9EDFF462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="740" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
     <t>${t.get("Rank")}</t>
   </si>
   <si>
-    <t>${l.customRank}</t>
-  </si>
-  <si>
-    <t>${l.customScoreComputed}</t>
+    <t>${l.score}</t>
+  </si>
+  <si>
+    <t>${l.scoreRank}</t>
   </si>
 </sst>
 </file>
@@ -1262,6 +1262,29 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1298,32 +1321,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1838,34 +1838,36 @@
   </sheetPr>
   <dimension ref="A1:X133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="13" width="7.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" style="3" customWidth="1"/>
-    <col min="16" max="18" width="7.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.1640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.1640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="7.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" style="3" customWidth="1"/>
+    <col min="16" max="18" width="7.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" style="1" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>21</v>
       </c>
@@ -1920,7 +1922,7 @@
       <c r="T2" s="65"/>
       <c r="U2" s="65"/>
     </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>23</v>
       </c>
@@ -1928,13 +1930,13 @@
       <c r="J3" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="140" t="s">
+      <c r="K3" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="129"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="68"/>
       <c r="R3" s="34" t="s">
@@ -1947,7 +1949,7 @@
       <c r="U3" s="70"/>
       <c r="V3" s="113"/>
     </row>
-    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="66" t="s">
         <v>30</v>
       </c>
@@ -1965,44 +1967,44 @@
       <c r="R4" s="34"/>
       <c r="S4" s="71"/>
     </row>
-    <row r="5" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="C6" s="9"/>
       <c r="H6" s="8"/>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="135" t="s">
+      <c r="K6" s="125" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="136"/>
-      <c r="M6" s="137"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="126"/>
       <c r="N6" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="135" t="s">
+      <c r="O6" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="137"/>
+      <c r="P6" s="141"/>
+      <c r="Q6" s="126"/>
       <c r="R6" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="S6" s="132" t="s">
+      <c r="S6" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="130" t="s">
+      <c r="T6" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="126" t="s">
+      <c r="U6" s="132" t="s">
         <v>95</v>
       </c>
-      <c r="V6" s="128" t="s">
+      <c r="V6" s="134" t="s">
         <v>96</v>
       </c>
       <c r="X6"/>
     </row>
-    <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>46</v>
       </c>
@@ -2015,10 +2017,10 @@
       <c r="D7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="135" t="s">
+      <c r="E7" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="137"/>
+      <c r="F7" s="126"/>
       <c r="G7" s="12" t="s">
         <v>40</v>
       </c>
@@ -2055,12 +2057,12 @@
       <c r="R7" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="133"/>
-      <c r="T7" s="131"/>
-      <c r="U7" s="127"/>
-      <c r="V7" s="129"/>
-    </row>
-    <row r="8" spans="1:24" s="29" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S7" s="139"/>
+      <c r="T7" s="137"/>
+      <c r="U7" s="133"/>
+      <c r="V7" s="135"/>
+    </row>
+    <row r="8" spans="1:24" s="29" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
         <v>65</v>
       </c>
@@ -2076,7 +2078,7 @@
       <c r="K8" s="77"/>
       <c r="V8" s="114"/>
     </row>
-    <row r="9" spans="1:24" s="29" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" s="29" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="75"/>
       <c r="C9" s="75"/>
@@ -2090,7 +2092,7 @@
       <c r="K9" s="77"/>
       <c r="V9" s="114"/>
     </row>
-    <row r="10" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="78" t="s">
         <v>62</v>
       </c>
@@ -2117,7 +2119,7 @@
       <c r="V10" s="115"/>
       <c r="X10"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -2139,7 +2141,7 @@
       <c r="W11"/>
       <c r="X11"/>
     </row>
-    <row r="12" spans="1:24" s="29" customFormat="1" ht="21.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" s="29" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>3</v>
       </c>
@@ -2152,10 +2154,10 @@
       <c r="D12" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="138" t="s">
+      <c r="E12" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="139"/>
+      <c r="F12" s="128"/>
       <c r="G12" s="73" t="s">
         <v>6</v>
       </c>
@@ -2199,13 +2201,13 @@
         <v>94</v>
       </c>
       <c r="U12" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="V12" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="V12" s="117" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2226,7 +2228,7 @@
       <c r="W13"/>
       <c r="X13"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2247,7 +2249,7 @@
       <c r="W14"/>
       <c r="X14"/>
     </row>
-    <row r="15" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15"/>
       <c r="G15"/>
       <c r="H15"/>
@@ -2265,7 +2267,7 @@
       <c r="W15"/>
       <c r="X15"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2286,14 +2288,14 @@
       <c r="W16"/>
       <c r="X16"/>
     </row>
-    <row r="17" spans="1:24" s="51" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" s="51" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
         <v>76</v>
       </c>
       <c r="J17" s="52"/>
       <c r="V17" s="118"/>
     </row>
-    <row r="18" spans="1:24" s="51" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" s="51" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="91"/>
@@ -2317,7 +2319,7 @@
       <c r="U18" s="97"/>
       <c r="V18" s="119"/>
     </row>
-    <row r="19" spans="1:24" s="109" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" s="109" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="100" t="s">
         <v>87</v>
       </c>
@@ -2364,7 +2366,7 @@
       <c r="V19" s="120"/>
       <c r="X19" s="102"/>
     </row>
-    <row r="20" spans="1:24" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="82" t="s">
         <v>66</v>
       </c>
@@ -2381,7 +2383,7 @@
       <c r="M20" s="85"/>
       <c r="V20" s="121"/>
     </row>
-    <row r="21" spans="1:24" s="87" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" s="87" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92" t="s">
         <v>67</v>
       </c>
@@ -2428,7 +2430,7 @@
       <c r="V21" s="122"/>
       <c r="X21" s="94"/>
     </row>
-    <row r="22" spans="1:24" s="87" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" s="87" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="87" t="s">
         <v>1</v>
       </c>
@@ -2449,7 +2451,7 @@
       <c r="V22" s="123"/>
       <c r="W22"/>
     </row>
-    <row r="23" spans="1:24" s="87" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" s="87" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="87" t="s">
         <v>73</v>
       </c>
@@ -2469,27 +2471,27 @@
       <c r="O23" s="83"/>
       <c r="V23" s="123"/>
     </row>
-    <row r="24" spans="1:24" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="141" t="s">
+      <c r="E24" s="130" t="s">
         <v>54</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="16"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="125" t="s">
+      <c r="J24" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="125"/>
+      <c r="K24" s="131"/>
       <c r="L24" s="15"/>
       <c r="N24" s="17"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="134" t="s">
+      <c r="Q24" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="R24" s="134"/>
+      <c r="R24" s="140"/>
       <c r="S24" s="49"/>
       <c r="T24" s="15"/>
       <c r="U24" s="13"/>
@@ -2499,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="37" t="s">
         <v>53</v>
@@ -2508,15 +2510,15 @@
         <v>28</v>
       </c>
       <c r="D25" s="18"/>
-      <c r="E25" s="141"/>
+      <c r="E25" s="130"/>
       <c r="F25" s="43" t="s">
         <v>82</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
-      <c r="J25" s="125"/>
-      <c r="K25" s="125"/>
+      <c r="J25" s="131"/>
+      <c r="K25" s="131"/>
       <c r="L25" s="43" t="s">
         <v>24</v>
       </c>
@@ -2524,8 +2526,8 @@
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
       <c r="P25" s="20"/>
-      <c r="Q25" s="134"/>
-      <c r="R25" s="134"/>
+      <c r="Q25" s="140"/>
+      <c r="R25" s="140"/>
       <c r="S25" s="43" t="s">
         <v>93</v>
       </c>
@@ -2535,7 +2537,7 @@
       <c r="W25"/>
       <c r="X25" s="18"/>
     </row>
-    <row r="26" spans="1:24" s="21" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" s="21" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
       <c r="B26" s="35"/>
       <c r="D26" s="39"/>
@@ -2556,17 +2558,17 @@
       <c r="V26" s="124"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="D27" s="1"/>
       <c r="E27" s="32"/>
       <c r="F27" s="15"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="125" t="s">
+      <c r="J27" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="125"/>
+      <c r="K27" s="131"/>
       <c r="M27"/>
       <c r="N27" s="1"/>
       <c r="O27" s="13"/>
@@ -2576,7 +2578,7 @@
       <c r="W27"/>
       <c r="X27"/>
     </row>
-    <row r="28" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="37" t="s">
         <v>57</v>
@@ -2594,8 +2596,8 @@
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="125"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="131"/>
       <c r="L28" s="43" t="s">
         <v>27</v>
       </c>
@@ -2609,7 +2611,7 @@
       <c r="W28"/>
       <c r="X28"/>
     </row>
-    <row r="29" spans="1:24" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
       <c r="B29" s="35"/>
       <c r="D29" s="39"/>
@@ -2627,7 +2629,7 @@
       <c r="V29" s="124"/>
       <c r="X29" s="39"/>
     </row>
-    <row r="30" spans="1:24" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="D30" s="1"/>
@@ -2645,7 +2647,7 @@
       <c r="W30"/>
       <c r="X30"/>
     </row>
-    <row r="31" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="37" t="s">
         <v>83</v>
@@ -2675,7 +2677,7 @@
       <c r="W31"/>
       <c r="X31"/>
     </row>
-    <row r="32" spans="1:24" s="21" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" s="21" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B32" s="22"/>
       <c r="D32" s="39"/>
       <c r="F32" s="16"/>
@@ -2693,7 +2695,7 @@
       <c r="S32" s="22"/>
       <c r="V32" s="124"/>
     </row>
-    <row r="33" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="33" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" s="2"/>
@@ -2705,324 +2707,319 @@
       <c r="S33" s="1"/>
       <c r="T33" s="13"/>
     </row>
-    <row r="34" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F34" s="1"/>
       <c r="U34" s="13"/>
     </row>
-    <row r="35" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F35" s="1"/>
       <c r="U35" s="13"/>
     </row>
-    <row r="36" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F36" s="1"/>
       <c r="U36" s="13"/>
     </row>
-    <row r="37" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F37" s="1"/>
       <c r="U37" s="13"/>
     </row>
-    <row r="38" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="38" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F38" s="1"/>
       <c r="U38" s="13"/>
     </row>
-    <row r="39" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D39" s="23"/>
       <c r="E39" s="23"/>
       <c r="F39" s="1"/>
       <c r="U39" s="13"/>
     </row>
-    <row r="40" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="40" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F40" s="1"/>
       <c r="U40" s="13"/>
     </row>
-    <row r="41" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="41" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F41" s="1"/>
       <c r="U41" s="13"/>
     </row>
-    <row r="42" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="42" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="43" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="44" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="45" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="46" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="4:21" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="117" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="119" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="121" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="122" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="123" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="124" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="125" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="126" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="127" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="128" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="129" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="130" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="131" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="132" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="133" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F133" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="J24:K25"/>
     <mergeCell ref="J27:K28"/>
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="V6:V7"/>
@@ -3031,6 +3028,11 @@
     <mergeCell ref="Q24:R25"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="J24:K25"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:D8">
     <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">

</xml_diff>

<commit_message>
wip assign ranks while computing medals
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/Score-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/Score-A4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5501B7BC-01B5-4F93-9A13-521C9EDFF462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6933D9FD-9D91-48DE-80B7-8FF89C665CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
     <t>${t.get("Rank")}</t>
   </si>
   <si>
-    <t>${l.score}</t>
-  </si>
-  <si>
-    <t>${l.scoreRank}</t>
+    <t>${l.categoryScore}</t>
+  </si>
+  <si>
+    <t>${l.categoryScoreRank}</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1262,50 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1284,46 +1324,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1839,7 +1839,7 @@
   <dimension ref="A1:X133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1930,13 +1930,13 @@
       <c r="J3" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="129" t="s">
+      <c r="K3" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="129"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140"/>
+      <c r="O3" s="140"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="68"/>
       <c r="R3" s="34" t="s">
@@ -1974,32 +1974,32 @@
       <c r="H6" s="8"/>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="125" t="s">
+      <c r="K6" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="141"/>
-      <c r="M6" s="126"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="137"/>
       <c r="N6" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="125" t="s">
+      <c r="O6" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="126"/>
+      <c r="P6" s="136"/>
+      <c r="Q6" s="137"/>
       <c r="R6" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="S6" s="138" t="s">
+      <c r="S6" s="132" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="136" t="s">
+      <c r="T6" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="132" t="s">
+      <c r="U6" s="126" t="s">
         <v>95</v>
       </c>
-      <c r="V6" s="134" t="s">
+      <c r="V6" s="128" t="s">
         <v>96</v>
       </c>
       <c r="X6"/>
@@ -2017,10 +2017,10 @@
       <c r="D7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="125" t="s">
+      <c r="E7" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="126"/>
+      <c r="F7" s="137"/>
       <c r="G7" s="12" t="s">
         <v>40</v>
       </c>
@@ -2057,10 +2057,10 @@
       <c r="R7" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="139"/>
-      <c r="T7" s="137"/>
-      <c r="U7" s="133"/>
-      <c r="V7" s="135"/>
+      <c r="S7" s="133"/>
+      <c r="T7" s="131"/>
+      <c r="U7" s="127"/>
+      <c r="V7" s="129"/>
     </row>
     <row r="8" spans="1:24" s="29" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
@@ -2154,10 +2154,10 @@
       <c r="D12" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="127" t="s">
+      <c r="E12" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="128"/>
+      <c r="F12" s="139"/>
       <c r="G12" s="73" t="s">
         <v>6</v>
       </c>
@@ -2475,23 +2475,23 @@
       <c r="A24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="130" t="s">
+      <c r="E24" s="141" t="s">
         <v>54</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="16"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="131" t="s">
+      <c r="J24" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="131"/>
+      <c r="K24" s="125"/>
       <c r="L24" s="15"/>
       <c r="N24" s="17"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="140" t="s">
+      <c r="Q24" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="R24" s="140"/>
+      <c r="R24" s="134"/>
       <c r="S24" s="49"/>
       <c r="T24" s="15"/>
       <c r="U24" s="13"/>
@@ -2510,15 +2510,15 @@
         <v>28</v>
       </c>
       <c r="D25" s="18"/>
-      <c r="E25" s="130"/>
+      <c r="E25" s="141"/>
       <c r="F25" s="43" t="s">
         <v>82</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
-      <c r="J25" s="131"/>
-      <c r="K25" s="131"/>
+      <c r="J25" s="125"/>
+      <c r="K25" s="125"/>
       <c r="L25" s="43" t="s">
         <v>24</v>
       </c>
@@ -2526,8 +2526,8 @@
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
       <c r="P25" s="20"/>
-      <c r="Q25" s="140"/>
-      <c r="R25" s="140"/>
+      <c r="Q25" s="134"/>
+      <c r="R25" s="134"/>
       <c r="S25" s="43" t="s">
         <v>93</v>
       </c>
@@ -2565,10 +2565,10 @@
       <c r="E27" s="32"/>
       <c r="F27" s="15"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="131" t="s">
+      <c r="J27" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="131"/>
+      <c r="K27" s="125"/>
       <c r="M27"/>
       <c r="N27" s="1"/>
       <c r="O27" s="13"/>
@@ -2596,8 +2596,8 @@
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
-      <c r="J28" s="131"/>
-      <c r="K28" s="131"/>
+      <c r="J28" s="125"/>
+      <c r="K28" s="125"/>
       <c r="L28" s="43" t="s">
         <v>27</v>
       </c>
@@ -3020,6 +3020,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="J24:K25"/>
     <mergeCell ref="J27:K28"/>
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="V6:V7"/>
@@ -3028,11 +3033,6 @@
     <mergeCell ref="Q24:R25"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="J24:K25"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:D8">
     <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">

</xml_diff>